<commit_message>
q4 complete; updated q2 parameters; results
</commit_message>
<xml_diff>
--- a/machinelearning/results.xlsx
+++ b/machinelearning/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngreenwald/Desktop/gmu/Spring-2019/cs-687/cs-687/machinelearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB68264-B17A-BC4C-807A-DF11D98F336E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D70AD6-8F88-A84D-895C-5A154AEB21CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15960" xr2:uid="{1BF98508-E7E3-1F43-8E01-F1C52225EE28}"/>
   </bookViews>
   <sheets>
     <sheet name="q2" sheetId="1" r:id="rId1"/>
     <sheet name="q3" sheetId="2" r:id="rId2"/>
+    <sheet name="q4" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>hidden layer</t>
   </si>
@@ -83,6 +84,18 @@
   </si>
   <si>
     <t>epochs</t>
+  </si>
+  <si>
+    <t>lots of variation even as epochs increase</t>
+  </si>
+  <si>
+    <t>was at .05 by 23,000</t>
+  </si>
+  <si>
+    <t>stuck at .14</t>
+  </si>
+  <si>
+    <t>.808 by 1000</t>
   </si>
 </sst>
 </file>
@@ -434,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DE1FAC-E1B9-D246-AA26-F8EA2D27791F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,74 +483,71 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>0.03</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>3.3</v>
+        <v>2.1610000000000002E-3</v>
       </c>
       <c r="F2">
-        <v>400</v>
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>1400</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>3.108E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="F3">
-        <v>669</v>
+        <v>12</v>
       </c>
       <c r="G3">
-        <v>111400</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>0.05</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>9.5769999999999994E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F4">
-        <v>330</v>
+        <v>7.06</v>
       </c>
       <c r="G4">
-        <v>57400</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -565,10 +575,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0.03</v>
@@ -577,88 +587,480 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>2.1610000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>8.18</v>
       </c>
       <c r="G6">
-        <v>1400</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C7">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7">
-        <v>1.884E-3</v>
+        <v>9.7000000000000003E-3</v>
       </c>
       <c r="F7">
-        <v>106</v>
+        <v>8.5</v>
       </c>
       <c r="G7">
-        <v>22200</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>1.0149999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F8">
-        <v>22.47</v>
+        <v>7.96</v>
       </c>
       <c r="G8">
-        <v>4500</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F9">
+        <v>9.31</v>
+      </c>
+      <c r="G9">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>0.03</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F10">
+        <v>10.43</v>
+      </c>
+      <c r="G10">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C11">
+        <v>0.02</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1.884E-3</v>
+      </c>
+      <c r="F11">
+        <v>106</v>
+      </c>
+      <c r="G11">
+        <v>22200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="F12">
+        <v>22.47</v>
+      </c>
+      <c r="G12">
+        <v>4500</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.05</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>1.56</v>
+      </c>
+      <c r="F13">
+        <v>59</v>
+      </c>
+      <c r="G13">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0.05</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0.26</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.05</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="F15">
+        <v>62</v>
+      </c>
+      <c r="G15">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
         <v>0.04</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>2E-3</v>
-      </c>
-      <c r="F9">
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="F16">
+        <v>99</v>
+      </c>
+      <c r="G16">
+        <v>17600</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>0.05</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>0.38</v>
+      </c>
+      <c r="F17">
+        <v>435</v>
+      </c>
+      <c r="G17">
+        <v>27800</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0.05</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18">
+        <v>230</v>
+      </c>
+      <c r="G18">
+        <v>30000</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>0.05</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>9.5769999999999994E-2</v>
+      </c>
+      <c r="F19">
+        <v>330</v>
+      </c>
+      <c r="G19">
+        <v>57400</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>0.03</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F20">
+        <v>462</v>
+      </c>
+      <c r="G20">
+        <v>84800</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>0.03</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>0.46</v>
+      </c>
+      <c r="F21">
+        <v>430</v>
+      </c>
+      <c r="G21">
+        <v>95500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0.03</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3.108E-2</v>
+      </c>
+      <c r="F22">
+        <v>669</v>
+      </c>
+      <c r="G22">
+        <v>111400</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>12</v>
       </c>
-      <c r="G9">
-        <v>2600</v>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>0.03</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F23">
+        <v>150</v>
+      </c>
+      <c r="G23">
+        <v>143000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>200</v>
+      </c>
+      <c r="C24">
+        <v>0.05</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>0.06</v>
+      </c>
+      <c r="F24">
+        <v>320</v>
+      </c>
+      <c r="G24">
+        <v>342000</v>
+      </c>
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>0.03</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>3.3</v>
+      </c>
+      <c r="F25">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:H26">
+    <sortCondition descending="1" ref="D2:D26"/>
+    <sortCondition ref="G2:G26"/>
+    <sortCondition ref="E2:E26"/>
+    <sortCondition ref="F2:F26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -669,7 +1071,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,4 +1303,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3EE0E4-73C3-604B-9977-405A17E08CFC}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>0.05</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>85.2</v>
+      </c>
+      <c r="G2">
+        <v>12.69</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>